<commit_message>
Fix xlsx templates and fix timeout for cdogs for AB#10862 and AB#10806
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/CovidReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/CovidReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laws/Projects/Health/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC0AC2F-FE1F-D749-A78A-8BB425281000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507CAA1F-C315-0A43-8D67-A14EDDF0CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
@@ -110,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -118,27 +118,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFAEAAAA"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFAEAAAA"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,27 +457,27 @@
     <col min="9" max="9" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -500,7 +491,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Fix xlsx templates and fix timeout for cdogs for AB#10862 and AB#10806 (#2553)
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/CovidReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/CovidReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laws/Projects/Health/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC0AC2F-FE1F-D749-A78A-8BB425281000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507CAA1F-C315-0A43-8D67-A14EDDF0CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
@@ -110,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -118,27 +118,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFAEAAAA"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFAEAAAA"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,27 +457,27 @@
     <col min="9" max="9" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -500,7 +491,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">

</xml_diff>